<commit_message>
addded working spice model
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
+    <sheet name="Power Supply" sheetId="2" r:id="rId2"/>
+    <sheet name="Gain" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>http://myhometheater.homestead.com/splcalculator.html</t>
   </si>
@@ -46,13 +48,104 @@
   </si>
   <si>
     <t>Power RMS (W)</t>
+  </si>
+  <si>
+    <t>https://www.parts-express.com/tc-6024-6-1-2-treated-paper-cone-woofer-with-foam-surround-4-ohm--299-2196</t>
+  </si>
+  <si>
+    <t>https://www.parts-express.com/goldwood-gw-8024-8-butyl-surround-woofer-4-ohm--290-356</t>
+  </si>
+  <si>
+    <t>Peak Output Voltage</t>
+  </si>
+  <si>
+    <t>Peak Output Current</t>
+  </si>
+  <si>
+    <r>
+      <t>Load Impedance (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω)</t>
+    </r>
+  </si>
+  <si>
+    <t>Tweeter</t>
+  </si>
+  <si>
+    <t>Average Output Power (W)</t>
+  </si>
+  <si>
+    <t>Transformer Voltage Regulation</t>
+  </si>
+  <si>
+    <t>Mains Voltage Variation</t>
+  </si>
+  <si>
+    <t>Drop-out voltage of LM3886</t>
+  </si>
+  <si>
+    <t>Minimum Gain</t>
+  </si>
+  <si>
+    <t>Woofer</t>
+  </si>
+  <si>
+    <r>
+      <t>Maximum Supply Voltage (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>±V)</t>
+    </r>
+  </si>
+  <si>
+    <t>Input Voltage Level</t>
+  </si>
+  <si>
+    <t>LM3886 Power Supply Requirements</t>
+  </si>
+  <si>
+    <t>Transformer Specifications</t>
+  </si>
+  <si>
+    <t>Voltage Regulation Error</t>
+  </si>
+  <si>
+    <t>Input (VAC)</t>
+  </si>
+  <si>
+    <t>Output (VAC)</t>
+  </si>
+  <si>
+    <t>Inductance Ratio</t>
+  </si>
+  <si>
+    <t>Rectified DC Voltage</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Tweeters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +157,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,10 +197,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -375,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,17 +499,17 @@
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -416,7 +526,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
       <c r="B6">
         <v>92.4</v>
       </c>
@@ -433,15 +546,46 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
       <c r="B7">
         <v>88.3</v>
       </c>
       <c r="C7">
         <v>60</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>106.1</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>93.4</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>110.4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -449,7 +593,230 @@
     <hyperlink ref="F6" r:id="rId1" xr:uid="{E978C543-6C32-4CC4-B95F-7525508C6FE7}"/>
     <hyperlink ref="F7" r:id="rId2" xr:uid="{73DD10AB-767F-4BDE-91A9-6FDB66FF532E}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{6A643506-44BF-43ED-8958-1D17814E5A81}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{FE8DAC70-499E-41F4-8E7B-6AF555A27CB3}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{ED5ACAA8-D4A7-4BC7-B19B-4624C59DBAC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEB1EA-E152-4802-8ABB-B4D06F75C74E}">
+  <dimension ref="B1:K19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>115</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <f>POWER((B5/C5), 2)</f>
+        <v>22.960069444444446</v>
+      </c>
+      <c r="E5">
+        <f>C5*SQRT(2)</f>
+        <v>33.941125496954285</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>120</v>
+      </c>
+      <c r="C6">
+        <f>B6/SQRT(D6)</f>
+        <v>25.043516133890467</v>
+      </c>
+      <c r="D6">
+        <v>22.96</v>
+      </c>
+      <c r="E6">
+        <f>C6*SQRT(2)</f>
+        <v>35.416880166057318</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+      <c r="E17">
+        <f>SQRT(2*C17*D17)</f>
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <f>SQRT(2*D17/C17)</f>
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <f>(E17+K$18)*(1+K$16)*(1+K$17)</f>
+        <v>28.248000000000001</v>
+      </c>
+      <c r="H17">
+        <f>SQRT(D17*C17)</f>
+        <v>14.142135623730951</v>
+      </c>
+      <c r="J17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>60</v>
+      </c>
+      <c r="E18">
+        <f>SQRT(2*C18*D18)</f>
+        <v>21.908902300206645</v>
+      </c>
+      <c r="F18">
+        <f>SQRT(2*D18/C18)</f>
+        <v>5.4772255750516612</v>
+      </c>
+      <c r="G18">
+        <f>(E18+K$18)*(1+K$16)*(1+K$17)</f>
+        <v>30.494778007343225</v>
+      </c>
+      <c r="H18">
+        <f>SQRT(D18*C18)</f>
+        <v>15.491933384829668</v>
+      </c>
+      <c r="J18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD76807-681C-4CA7-A650-2C811CF779EA}">
+  <dimension ref="B1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added power simulation and calculations
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECB87E4-68AF-4EEA-AFF6-940144F05639}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>http://myhometheater.homestead.com/splcalculator.html</t>
   </si>
@@ -140,12 +141,129 @@
   <si>
     <t>Tweeters</t>
   </si>
+  <si>
+    <t>Voltage Given Power</t>
+  </si>
+  <si>
+    <t>Power Given Voltage</t>
+  </si>
+  <si>
+    <t>https://www.parts-express.com/goldwood-gw-s650-4-6-1-2-poly-cone-woofer-4-ohm--290-308</t>
+  </si>
+  <si>
+    <t>Power Dissipation</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DMAX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Vcc*2/2*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>π</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">cc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= |V+| + |V-|</t>
+    </r>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>We have a set supply (~35v), which gives us the output power at that voltage</t>
+  </si>
+  <si>
+    <t>We can set our gain accordingly, to limit output voltage, and therefore limit power to speaker</t>
+  </si>
+  <si>
+    <t>OR we can select a smaller transformer and smaller speakers</t>
+  </si>
+  <si>
+    <t>P average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +293,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -197,12 +337,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -220,6 +363,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E40B576A-DE59-40DA-9FC1-FEF71E095769}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6848475" y="1038225"/>
+          <a:ext cx="1057275" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,9 +748,6 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
       <c r="B7">
         <v>88.3</v>
       </c>
@@ -586,6 +784,40 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F9" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>90</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>107</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>88.3</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>105.3</v>
       </c>
     </row>
   </sheetData>
@@ -602,15 +834,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEB1EA-E152-4802-8ABB-B4D06F75C74E}">
-  <dimension ref="B1:K19"/>
+  <dimension ref="B1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -665,7 +897,7 @@
         <v>33.941125496954285</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>120</v>
       </c>
@@ -680,12 +912,36 @@
         <f>C6*SQRT(2)</f>
         <v>35.416880166057318</v>
       </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>117</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <f>POWER((B7/C7), 2)</f>
+        <v>28.283057851239672</v>
+      </c>
+      <c r="E7">
+        <f>C7*SQRT(2)</f>
+        <v>31.112698372208094</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3"/>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
@@ -710,7 +966,7 @@
         <v>16</v>
       </c>
       <c r="K16">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -733,7 +989,7 @@
       </c>
       <c r="G17">
         <f>(E17+K$18)*(1+K$16)*(1+K$17)</f>
-        <v>28.248000000000001</v>
+        <v>29.040000000000006</v>
       </c>
       <c r="H17">
         <f>SQRT(D17*C17)</f>
@@ -766,7 +1022,7 @@
       </c>
       <c r="G18">
         <f>(E18+K$18)*(1+K$16)*(1+K$17)</f>
-        <v>30.494778007343225</v>
+        <v>31.349771783250045</v>
       </c>
       <c r="H18">
         <f>SQRT(D18*C18)</f>
@@ -787,13 +1043,141 @@
         <v>1</v>
       </c>
     </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f>POWER(E23,2)/8</f>
+        <v>79.822553163157323</v>
+      </c>
+      <c r="E23">
+        <f>(G23/((1+K$16)*(1+K$17))) - 4</f>
+        <v>25.270148897568028</v>
+      </c>
+      <c r="F23">
+        <f>SQRT((2*D23)/C23)</f>
+        <v>6.3175372243920069</v>
+      </c>
+      <c r="G23">
+        <f>E6</f>
+        <v>35.416880166057318</v>
+      </c>
+      <c r="H23">
+        <f>SQRT(D23*C23)</f>
+        <v>17.868693647064109</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <f>POWER(E24,2)/8</f>
+        <v>58.919549552626165</v>
+      </c>
+      <c r="E24">
+        <f>(G24/((1+K$16)*(1+K$17))) - 4</f>
+        <v>21.710743801652889</v>
+      </c>
+      <c r="F24">
+        <f>SQRT((2*D24)/C24)</f>
+        <v>5.4276859504132222</v>
+      </c>
+      <c r="G24">
+        <v>31.11</v>
+      </c>
+      <c r="H24">
+        <f>SQRT(D24*C24)</f>
+        <v>15.351814166752561</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="27" spans="2:11" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f>POWER(2*E6,2)/(2*POWER(PI(),2)*$C$24)</f>
+        <v>63.546386953382587</v>
+      </c>
+      <c r="D28">
+        <f>(E23/C23)*(E6*2/PI() - E23/2)</f>
+        <v>62.619503139227582</v>
+      </c>
+      <c r="J28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f>POWER(2*E7,2)/(2*POWER(PI(),2)*$C$24)</f>
+        <v>49.039452882891489</v>
+      </c>
+      <c r="J29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -801,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD76807-681C-4CA7-A650-2C811CF779EA}">
   <dimension ref="B1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Altium PCB project and libraries
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECB87E4-68AF-4EEA-AFF6-940144F05639}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903765D2-18C8-4F8F-B0BC-69DFA978ED09}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>http://myhometheater.homestead.com/splcalculator.html</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Tweeters</t>
   </si>
   <si>
     <t>Voltage Given Power</t>
@@ -244,19 +241,54 @@
     </r>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>We have a set supply (~35v), which gives us the output power at that voltage</t>
-  </si>
-  <si>
-    <t>We can set our gain accordingly, to limit output voltage, and therefore limit power to speaker</t>
-  </si>
-  <si>
-    <t>OR we can select a smaller transformer and smaller speakers</t>
-  </si>
-  <si>
-    <t>P average</t>
+    <t>Ri</t>
+  </si>
+  <si>
+    <t>Av</t>
+  </si>
+  <si>
+    <t>Vout (RMS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vout (MAX) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P (RMS) </t>
+  </si>
+  <si>
+    <t>P (Max)</t>
+  </si>
+  <si>
+    <r>
+      <t>Rf (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω)</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.parts-express.com/goldwood-gw-6024-6-1-2-butyl-surround-woofer-4-ohm--290-351</t>
+  </si>
+  <si>
+    <t>I (Max)</t>
+  </si>
+  <si>
+    <t>1khz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>31.14 V</t>
+  </si>
+  <si>
+    <t>Total Power (Max)</t>
   </si>
 </sst>
 </file>
@@ -337,16 +369,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -686,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,14 +832,11 @@
       <c r="E10">
         <v>107</v>
       </c>
-      <c r="F10" t="s">
-        <v>34</v>
+      <c r="F10" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
       <c r="B11">
         <v>88.3</v>
       </c>
@@ -818,6 +848,26 @@
       </c>
       <c r="E11">
         <v>105.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>89.5</v>
+      </c>
+      <c r="C12">
+        <v>60</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>107.3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -827,6 +877,8 @@
     <hyperlink ref="B2" r:id="rId3" xr:uid="{6A643506-44BF-43ED-8958-1D17814E5A81}"/>
     <hyperlink ref="F8" r:id="rId4" xr:uid="{FE8DAC70-499E-41F4-8E7B-6AF555A27CB3}"/>
     <hyperlink ref="F9" r:id="rId5" xr:uid="{ED5ACAA8-D4A7-4BC7-B19B-4624C59DBAC5}"/>
+    <hyperlink ref="F12" r:id="rId6" xr:uid="{19074139-D16F-424A-9E61-337C93775B88}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{801E6B22-FB02-4EBE-AB0B-E2CEF6497134}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -834,10 +886,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEB1EA-E152-4802-8ABB-B4D06F75C74E}">
-  <dimension ref="B1:K30"/>
+  <dimension ref="B1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,10 +906,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -913,7 +965,7 @@
         <v>35.416880166057318</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -932,15 +984,31 @@
         <v>31.112698372208094</v>
       </c>
     </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>120</v>
+      </c>
+      <c r="C8">
+        <f>B8/SQRT(D8)</f>
+        <v>22.564125640873733</v>
+      </c>
+      <c r="D8">
+        <v>28.283000000000001</v>
+      </c>
+      <c r="E8">
+        <f>C8*SQRT(2)</f>
+        <v>31.91049250441414</v>
+      </c>
+    </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
@@ -970,9 +1038,6 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
       <c r="C17">
         <v>4</v>
       </c>
@@ -1003,9 +1068,6 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
       <c r="C18">
         <v>4</v>
       </c>
@@ -1036,6 +1098,28 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <f>SQRT(2*C19*D19)</f>
+        <v>17.888543819998318</v>
+      </c>
+      <c r="F19">
+        <f>SQRT(2*D19/C19)</f>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="G19">
+        <f>(E19+K$18)*(1+K$16)*(1+K$17)</f>
+        <v>26.485138022197972</v>
+      </c>
+      <c r="H19">
+        <f>SQRT(D19*C19)</f>
+        <v>12.649110640673518</v>
+      </c>
       <c r="J19" t="s">
         <v>22</v>
       </c>
@@ -1045,7 +1129,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1067,107 +1151,156 @@
       <c r="H22" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23">
         <f>POWER(E23,2)/8</f>
-        <v>79.822553163157323</v>
+        <v>62.562743323543458</v>
       </c>
       <c r="E23">
         <f>(G23/((1+K$16)*(1+K$17))) - 4</f>
-        <v>25.270148897568028</v>
+        <v>22.371900826446279</v>
       </c>
       <c r="F23">
         <f>SQRT((2*D23)/C23)</f>
-        <v>6.3175372243920069</v>
+        <v>5.5929752066115697</v>
       </c>
       <c r="G23">
+        <v>31.91</v>
+      </c>
+      <c r="H23">
+        <f>SQRT(D23*C23)</f>
+        <v>15.81932278241309</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <f>POWER(E24,2)/8</f>
+        <v>62.562743323543458</v>
+      </c>
+      <c r="E24">
+        <f>(G24/((1+K$16)*(1+K$17))) - 4</f>
+        <v>22.371900826446279</v>
+      </c>
+      <c r="F24">
+        <f>SQRT((2*D24)/C24)</f>
+        <v>5.5929752066115697</v>
+      </c>
+      <c r="G24">
+        <v>31.91</v>
+      </c>
+      <c r="H24">
+        <f>SQRT(D24*C24)</f>
+        <v>15.81932278241309</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <f>POWER(E25,2)/8</f>
+        <v>79.823178829997943</v>
+      </c>
+      <c r="E25">
+        <f>(G25/((1+K$16)*(1+K$17))) - 4</f>
+        <v>25.270247933884296</v>
+      </c>
+      <c r="F25">
+        <f>SQRT((2*D25)/C25)</f>
+        <v>6.3175619834710739</v>
+      </c>
+      <c r="G25">
+        <v>35.417000000000002</v>
+      </c>
+      <c r="H25">
+        <f>SQRT(D25*C25)</f>
+        <v>17.868763676314927</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <f>POWER(E26,2)/8</f>
+        <v>79.823178829997943</v>
+      </c>
+      <c r="E26">
+        <f>(G26/((1+K$16)*(1+K$17))) - 4</f>
+        <v>25.270247933884296</v>
+      </c>
+      <c r="F26">
+        <f>SQRT((2*D26)/C26)</f>
+        <v>5.6505992188438894</v>
+      </c>
+      <c r="G26">
+        <v>35.417000000000002</v>
+      </c>
+      <c r="H26">
+        <f>SQRT(D26*C26)</f>
+        <v>19.977885127059611</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30">
         <f>E6</f>
         <v>35.416880166057318</v>
       </c>
-      <c r="H23">
-        <f>SQRT(D23*C23)</f>
-        <v>17.868693647064109</v>
-      </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <f>POWER(E24,2)/8</f>
-        <v>58.919549552626165</v>
-      </c>
-      <c r="E24">
-        <f>(G24/((1+K$16)*(1+K$17))) - 4</f>
-        <v>21.710743801652889</v>
-      </c>
-      <c r="F24">
-        <f>SQRT((2*D24)/C24)</f>
-        <v>5.4276859504132222</v>
-      </c>
-      <c r="G24">
-        <v>31.11</v>
-      </c>
-      <c r="H24">
-        <f>SQRT(D24*C24)</f>
-        <v>15.351814166752561</v>
-      </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="27" spans="2:11" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" t="s">
-        <v>42</v>
-      </c>
-      <c r="J27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C28">
+      <c r="C30">
         <f>POWER(2*E6,2)/(2*POWER(PI(),2)*$C$24)</f>
         <v>63.546386953382587</v>
       </c>
-      <c r="D28">
-        <f>(E23/C23)*(E6*2/PI() - E23/2)</f>
-        <v>62.619503139227582</v>
-      </c>
-      <c r="J28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29">
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f t="shared" ref="B31:B32" si="0">E7</f>
+        <v>31.112698372208094</v>
+      </c>
+      <c r="C31">
         <f>POWER(2*E7,2)/(2*POWER(PI(),2)*$C$24)</f>
         <v>49.039452882891489</v>
       </c>
-      <c r="J29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J30" t="s">
-        <v>41</v>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>31.91049250441414</v>
+      </c>
+      <c r="C32">
+        <f>POWER(2*E8,2)/(2*POWER(PI(),2)*$C$24)</f>
+        <v>51.586643724133381</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f>C30*4 + (Gain!G10*2) + (Gain!G19*2)</f>
+        <v>564.5855478135303</v>
       </c>
     </row>
   </sheetData>
@@ -1183,24 +1316,514 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD76807-681C-4CA7-A650-2C811CF779EA}">
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="3"/>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>100000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <f>$C$3/(B6-1)</f>
+        <v>6666.666666666667</v>
+      </c>
+      <c r="D6">
+        <v>11.32</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E10" si="0">D6*SQRT(2)</f>
+        <v>16.008897526063439</v>
+      </c>
+      <c r="F6">
+        <f>G6/SQRT(2)</f>
+        <v>45.233620792503444</v>
+      </c>
+      <c r="G6">
+        <v>63.97</v>
+      </c>
+      <c r="H6">
+        <f>G6/E6</f>
+        <v>3.9959028968642611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>B6+0.2</f>
+        <v>16.2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C10" si="1">$C$3/(B7-1)</f>
+        <v>6578.9473684210525</v>
+      </c>
+      <c r="D7">
+        <v>11.45</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>16.192745289171938</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F10" si="2">G7/SQRT(2)</f>
+        <v>46.386204845837511</v>
+      </c>
+      <c r="G7">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H22" si="3">G7/E7</f>
+        <v>4.0511969297674684</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" ref="B8:B10" si="4">B7+0.2</f>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>6493.5064935064938</v>
+      </c>
+      <c r="D8">
+        <v>11.6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>16.404877323527902</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>47.52464676354785</v>
+      </c>
+      <c r="G8">
+        <v>67.209999999999994</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>4.0969523072024012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" si="4"/>
+        <v>16.599999999999998</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>6410.2564102564111</v>
+      </c>
+      <c r="D9">
+        <v>11.74</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>16.602867222260137</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>48.69137295250566</v>
+      </c>
+      <c r="G9">
+        <v>68.86</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>4.1474764014059335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="4"/>
+        <v>16.799999999999997</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>6329.1139240506336</v>
+      </c>
+      <c r="D10">
+        <v>11.88</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>16.800857120992372</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>49.893454480522792</v>
+      </c>
+      <c r="G10">
+        <v>70.56</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>4.1997857306837361</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C16" si="5">$C$3/(B11-1)</f>
+        <v>6250</v>
+      </c>
+      <c r="D11">
+        <v>12.02</v>
+      </c>
+      <c r="E11">
+        <f>D11*SQRT(2)</f>
+        <v>16.998847019724604</v>
+      </c>
+      <c r="F11">
+        <f>G11/SQRT(2)</f>
+        <v>51.07432280510433</v>
+      </c>
+      <c r="G11">
+        <v>72.23</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>4.249111714234969</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>17.5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="5"/>
+        <v>6060.606060606061</v>
+      </c>
+      <c r="D12">
+        <v>12.37</v>
+      </c>
+      <c r="E12">
+        <f>D12*SQRT(2)</f>
+        <v>17.493821766555186</v>
+      </c>
+      <c r="F12">
+        <f>G12/SQRT(2)</f>
+        <v>54.114881964206482</v>
+      </c>
+      <c r="G12">
+        <v>76.53</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>4.3746873051096591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>B12+0.1</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="5"/>
+        <v>6024.0963855421678</v>
+      </c>
+      <c r="D13">
+        <v>12.44</v>
+      </c>
+      <c r="E13">
+        <f>D13*SQRT(2)</f>
+        <v>17.592816715921302</v>
+      </c>
+      <c r="F13">
+        <f>G13/SQRT(2)</f>
+        <v>54.751278067274377</v>
+      </c>
+      <c r="G13">
+        <v>77.430000000000007</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>4.4012281404561397</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" ref="B14:B16" si="6">B13+0.1</f>
+        <v>17.700000000000003</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="5"/>
+        <v>5988.0239520958075</v>
+      </c>
+      <c r="E14">
+        <f>D14*SQRT(2)</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F21" si="7">G14/SQRT(2)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" si="6"/>
+        <v>17.800000000000004</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="5"/>
+        <v>5952.3809523809505</v>
+      </c>
+      <c r="D15">
+        <v>12.59</v>
+      </c>
+      <c r="E15">
+        <f>D15*SQRT(2)</f>
+        <v>17.804948750277269</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="7"/>
+        <v>55.981643866538967</v>
+      </c>
+      <c r="G15">
+        <v>79.17</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>4.4465165898760093</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" si="6"/>
+        <v>17.900000000000006</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="5"/>
+        <v>5917.1597633136071</v>
+      </c>
+      <c r="E16">
+        <f>D16*SQRT(2)</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H16" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <f>$C$3/(B17-1)</f>
+        <v>5882.3529411764703</v>
+      </c>
+      <c r="D17">
+        <v>12.73</v>
+      </c>
+      <c r="E17">
+        <f>D17*SQRT(2)</f>
+        <v>18.002938649009501</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="7"/>
+        <v>57.289791411734072</v>
+      </c>
+      <c r="G17">
+        <v>81.02</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>4.500376387410375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>B17+0.2</f>
+        <v>18.2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:C21" si="8">$C$3/(B18-1)</f>
+        <v>5813.9534883720935</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:E21" si="9">D18*SQRT(2)</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H18" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ref="B19:B21" si="10">B18+0.2</f>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="8"/>
+        <v>5747.1264367816093</v>
+      </c>
+      <c r="D19">
+        <v>13.01</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="9"/>
+        <v>18.398918446473967</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>59.849517959629381</v>
+      </c>
+      <c r="G19">
+        <v>84.64</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>4.6002704042758937</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="10"/>
+        <v>18.599999999999998</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="8"/>
+        <v>5681.8181818181829</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H20" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="10"/>
+        <v>18.799999999999997</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="8"/>
+        <v>5617.9775280898884</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H21" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <f>$C$3/(B22-1)</f>
+        <v>5555.5555555555557</v>
+      </c>
+      <c r="D22">
+        <v>13.43</v>
+      </c>
+      <c r="E22">
+        <f>D22*SQRT(2)</f>
+        <v>18.992888142670669</v>
+      </c>
+      <c r="F22">
+        <f>G22/SQRT(2)</f>
+        <v>63.802244866462182</v>
+      </c>
+      <c r="G22">
+        <v>90.23</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>4.7507256043531036</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V27" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added simulation and calculations for low pass filter
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -3,14 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903765D2-18C8-4F8F-B0BC-69DFA978ED09}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A5A219-12A2-477D-8CD1-EEBB0DF41AEF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
     <sheet name="Power Supply" sheetId="2" r:id="rId2"/>
     <sheet name="Gain" sheetId="3" r:id="rId3"/>
+    <sheet name="Mute Attenuation" sheetId="4" r:id="rId4"/>
+    <sheet name="Optional Components" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>http://myhometheater.homestead.com/splcalculator.html</t>
   </si>
@@ -289,6 +291,91 @@
   </si>
   <si>
     <t>Total Power (Max)</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">M   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> for </t>
+  </si>
+  <si>
+    <t>gain (dB)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>R2 resistor in op amp feedback</t>
+  </si>
+  <si>
+    <t>See 'Gain' sheet</t>
+  </si>
+  <si>
+    <t>Ci</t>
+  </si>
+  <si>
+    <t>Low-frequency roll-off in series with Ri</t>
+  </si>
+  <si>
+    <r>
+      <t>1/(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>π*Ri*f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -369,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -380,6 +467,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,6 +541,55 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>427119</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>18902</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA83D6F-E080-47AD-ABD9-E6DFDF741875}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="571500" y="171450"/>
+          <a:ext cx="12047619" cy="1180952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -888,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEB1EA-E152-4802-8ABB-B4D06F75C74E}">
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1438,7 @@
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35">
-        <f>C30*4 + (Gain!G10*2) + (Gain!G19*2)</f>
+        <f>C30*4 + (Gain!H10*2) + (Gain!H19*2)</f>
         <v>564.5855478135303</v>
       </c>
     </row>
@@ -1316,510 +1455,776 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD76807-681C-4CA7-A650-2C811CF779EA}">
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D1" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>100000</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>46</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>38</v>
       </c>
       <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>40</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>41</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>16</v>
       </c>
       <c r="C6">
-        <f>$C$3/(B6-1)</f>
+        <f>LOG(B6,10)*20</f>
+        <v>24.082399653118493</v>
+      </c>
+      <c r="D6">
+        <f>$D$3/(B6-1)</f>
         <v>6666.666666666667</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>11.32</v>
       </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E10" si="0">D6*SQRT(2)</f>
+      <c r="F6">
+        <f t="shared" ref="F6:F10" si="0">E6*SQRT(2)</f>
         <v>16.008897526063439</v>
       </c>
-      <c r="F6">
-        <f>G6/SQRT(2)</f>
+      <c r="G6">
+        <f>H6/SQRT(2)</f>
         <v>45.233620792503444</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>63.97</v>
       </c>
-      <c r="H6">
-        <f>G6/E6</f>
+      <c r="I6">
+        <f>H6/F6</f>
         <v>3.9959028968642611</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>B6+0.2</f>
         <v>16.2</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C10" si="1">$C$3/(B7-1)</f>
+        <f t="shared" ref="C7:C32" si="1">LOG(B7,10)*20</f>
+        <v>24.190300290852615</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D10" si="2">$D$3/(B7-1)</f>
         <v>6578.9473684210525</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>11.45</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>16.192745289171938</v>
       </c>
-      <c r="F7">
-        <f t="shared" ref="F7:F10" si="2">G7/SQRT(2)</f>
+      <c r="G7">
+        <f t="shared" ref="G7:G10" si="3">H7/SQRT(2)</f>
         <v>46.386204845837511</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>65.599999999999994</v>
       </c>
-      <c r="H7">
-        <f t="shared" ref="H7:H22" si="3">G7/E7</f>
+      <c r="I7">
+        <f t="shared" ref="I7:I22" si="4">H7/F7</f>
         <v>4.0511969297674684</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
-        <f t="shared" ref="B8:B10" si="4">B7+0.2</f>
+        <f t="shared" ref="B8:B10" si="5">B7+0.2</f>
         <v>16.399999999999999</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
+        <v>24.296876960953956</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
         <v>6493.5064935064938</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>11.6</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>16.404877323527902</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
+      <c r="G8">
+        <f t="shared" si="3"/>
         <v>47.52464676354785</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>67.209999999999994</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="3"/>
+      <c r="I8">
+        <f t="shared" si="4"/>
         <v>4.0969523072024012</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16.599999999999998</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
+        <v>24.402161760801096</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
         <v>6410.2564102564111</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>11.74</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>16.602867222260137</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
+      <c r="G9">
+        <f t="shared" si="3"/>
         <v>48.69137295250566</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>68.86</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="3"/>
+      <c r="I9">
+        <f t="shared" si="4"/>
         <v>4.1474764014059335</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16.799999999999997</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
+        <v>24.506185634517252</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
         <v>6329.1139240506336</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>11.88</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <f t="shared" si="0"/>
         <v>16.800857120992372</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
+      <c r="G10">
+        <f t="shared" si="3"/>
         <v>49.893454480522792</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>70.56</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="3"/>
+      <c r="I10">
+        <f t="shared" si="4"/>
         <v>4.1997857306837361</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>17</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C16" si="5">$C$3/(B11-1)</f>
+        <f t="shared" si="1"/>
+        <v>24.608978427565479</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D16" si="6">$D$3/(B11-1)</f>
         <v>6250</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>12.02</v>
       </c>
-      <c r="E11">
-        <f>D11*SQRT(2)</f>
+      <c r="F11">
+        <f>E11*SQRT(2)</f>
         <v>16.998847019724604</v>
       </c>
-      <c r="F11">
-        <f>G11/SQRT(2)</f>
+      <c r="G11">
+        <f>H11/SQRT(2)</f>
         <v>51.07432280510433</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>72.23</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="3"/>
+      <c r="I11">
+        <f t="shared" si="4"/>
         <v>4.249111714234969</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>17.5</v>
       </c>
       <c r="C12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
+        <v>24.860760973725888</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="6"/>
         <v>6060.606060606061</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>12.37</v>
       </c>
-      <c r="E12">
-        <f>D12*SQRT(2)</f>
+      <c r="F12">
+        <f>E12*SQRT(2)</f>
         <v>17.493821766555186</v>
       </c>
-      <c r="F12">
-        <f>G12/SQRT(2)</f>
+      <c r="G12">
+        <f>H12/SQRT(2)</f>
         <v>54.114881964206482</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>76.53</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="3"/>
+      <c r="I12">
+        <f t="shared" si="4"/>
         <v>4.3746873051096591</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>B12+0.1</f>
         <v>17.600000000000001</v>
       </c>
       <c r="C13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
+        <v>24.910253356282993</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="6"/>
         <v>6024.0963855421678</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>12.44</v>
       </c>
-      <c r="E13">
-        <f>D13*SQRT(2)</f>
+      <c r="F13">
+        <f>E13*SQRT(2)</f>
         <v>17.592816715921302</v>
       </c>
-      <c r="F13">
-        <f>G13/SQRT(2)</f>
+      <c r="G13">
+        <f>H13/SQRT(2)</f>
         <v>54.751278067274377</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>77.430000000000007</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="3"/>
+      <c r="I13">
+        <f t="shared" si="4"/>
         <v>4.4012281404561397</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
-        <f t="shared" ref="B14:B16" si="6">B13+0.1</f>
+        <f t="shared" ref="B14:B16" si="7">B13+0.1</f>
         <v>17.700000000000003</v>
       </c>
       <c r="C14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
+        <v>24.959465327236131</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="6"/>
         <v>5988.0239520958075</v>
       </c>
-      <c r="E14">
-        <f>D14*SQRT(2)</f>
+      <c r="F14">
+        <f>E14*SQRT(2)</f>
         <v>0</v>
       </c>
-      <c r="F14">
-        <f t="shared" ref="F14:F21" si="7">G14/SQRT(2)</f>
+      <c r="G14">
+        <f t="shared" ref="G14:G21" si="8">H14/SQRT(2)</f>
         <v>0</v>
       </c>
-      <c r="H14" t="e">
-        <f t="shared" si="3"/>
+      <c r="I14" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
+        <f t="shared" si="7"/>
+        <v>17.800000000000004</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>25.008400046177876</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="6"/>
-        <v>17.800000000000004</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="5"/>
         <v>5952.3809523809505</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>12.59</v>
       </c>
-      <c r="E15">
-        <f>D15*SQRT(2)</f>
+      <c r="F15">
+        <f>E15*SQRT(2)</f>
         <v>17.804948750277269</v>
       </c>
-      <c r="F15">
+      <c r="G15">
+        <f t="shared" si="8"/>
+        <v>55.981643866538967</v>
+      </c>
+      <c r="H15">
+        <v>79.17</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>4.4465165898760093</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16">
         <f t="shared" si="7"/>
-        <v>55.981643866538967</v>
-      </c>
-      <c r="G15">
-        <v>79.17</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="3"/>
-        <v>4.4465165898760093</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16">
+        <v>17.900000000000006</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>25.057060619597863</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="6"/>
-        <v>17.900000000000006</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="5"/>
         <v>5917.1597633136071</v>
       </c>
-      <c r="E16">
-        <f>D16*SQRT(2)</f>
+      <c r="F16">
+        <f>E16*SQRT(2)</f>
         <v>0</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="7"/>
+      <c r="G16">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H16" t="e">
-        <f t="shared" si="3"/>
+      <c r="I16" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>18</v>
       </c>
       <c r="C17">
-        <f>$C$3/(B17-1)</f>
+        <f t="shared" si="1"/>
+        <v>25.105450102066115</v>
+      </c>
+      <c r="D17">
+        <f>$D$3/(B17-1)</f>
         <v>5882.3529411764703</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>12.73</v>
       </c>
-      <c r="E17">
-        <f>D17*SQRT(2)</f>
+      <c r="F17">
+        <f>E17*SQRT(2)</f>
         <v>18.002938649009501</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="7"/>
+      <c r="G17">
+        <f t="shared" si="8"/>
         <v>57.289791411734072</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>81.02</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="3"/>
+      <c r="I17">
+        <f t="shared" si="4"/>
         <v>4.500376387410375</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>B17+0.2</f>
         <v>18.2</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:C21" si="8">$C$3/(B18-1)</f>
+        <f t="shared" si="1"/>
+        <v>25.201427759701495</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:D21" si="9">$D$3/(B18-1)</f>
         <v>5813.9534883720935</v>
       </c>
-      <c r="E18">
-        <f t="shared" ref="E18:E21" si="9">D18*SQRT(2)</f>
+      <c r="F18">
+        <f t="shared" ref="F18:F21" si="10">E18*SQRT(2)</f>
         <v>0</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="7"/>
+      <c r="G18">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H18" t="e">
-        <f t="shared" si="3"/>
+      <c r="I18" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:B21" si="10">B18+0.2</f>
+        <f t="shared" ref="B19:B21" si="11">B18+0.2</f>
         <v>18.399999999999999</v>
       </c>
       <c r="C19">
+        <f t="shared" si="1"/>
+        <v>25.296356460190729</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="9"/>
+        <v>5747.1264367816093</v>
+      </c>
+      <c r="E19">
+        <v>13.01</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="10"/>
+        <v>18.398918446473967</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="8"/>
-        <v>5747.1264367816093</v>
-      </c>
-      <c r="D19">
-        <v>13.01</v>
-      </c>
-      <c r="E19">
+        <v>59.849517959629381</v>
+      </c>
+      <c r="H19">
+        <v>84.64</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>4.6002704042758937</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="11"/>
+        <v>18.599999999999998</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>25.390258884358321</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="9"/>
-        <v>18.398918446473967</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="7"/>
-        <v>59.849517959629381</v>
-      </c>
-      <c r="G19">
-        <v>84.64</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="3"/>
-        <v>4.6002704042758937</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B20">
+        <v>5681.8181818181829</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="10"/>
-        <v>18.599999999999998</v>
-      </c>
-      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="8"/>
-        <v>5681.8181818181829</v>
-      </c>
-      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="11"/>
+        <v>18.799999999999997</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>25.483156985273592</v>
+      </c>
+      <c r="D21">
         <f t="shared" si="9"/>
+        <v>5617.9775280898884</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="7"/>
+      <c r="G21">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H20" t="e">
-        <f t="shared" si="3"/>
+      <c r="I21" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <f t="shared" si="10"/>
-        <v>18.799999999999997</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="8"/>
-        <v>5617.9775280898884</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H21" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>19</v>
       </c>
       <c r="C22">
-        <f>$C$3/(B22-1)</f>
+        <f t="shared" si="1"/>
+        <v>25.575072019056577</v>
+      </c>
+      <c r="D22">
+        <f>$D$3/(B22-1)</f>
         <v>5555.5555555555557</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>13.43</v>
       </c>
-      <c r="E22">
-        <f>D22*SQRT(2)</f>
+      <c r="F22">
+        <f>E22*SQRT(2)</f>
         <v>18.992888142670669</v>
       </c>
-      <c r="F22">
-        <f>G22/SQRT(2)</f>
+      <c r="G22">
+        <f>H22/SQRT(2)</f>
         <v>63.802244866462182</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>90.23</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="3"/>
+      <c r="I22">
+        <f t="shared" si="4"/>
         <v>4.7507256043531036</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="V27" t="s">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C25">
+        <f>LOG(B25,10)*20</f>
+        <v>0.82785370316450146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>2.1</v>
+      </c>
+      <c r="C26">
+        <f>LOG(B26,10)*20</f>
+        <v>6.4443858946783852</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>3.1</v>
+      </c>
+      <c r="C27">
+        <f>LOG(B27,10)*20</f>
+        <v>9.8272338766854528</v>
+      </c>
+      <c r="W27" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C28">
+        <f>LOG(B28,10)*20</f>
+        <v>12.255677134394709</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C29">
+        <f>LOG(B29,10)*20</f>
+        <v>14.151403521958725</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>6.1</v>
+      </c>
+      <c r="C30">
+        <f>LOG(B30,10)*20</f>
+        <v>15.706596700215339</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>7.1</v>
+      </c>
+      <c r="C31">
+        <f>LOG(B31,10)*20</f>
+        <v>17.025166974381506</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>8.1</v>
+      </c>
+      <c r="C32">
+        <f>LOG(B32,10)*20</f>
+        <v>18.169700377572994</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>9.1</v>
+      </c>
+      <c r="C33">
+        <f>LOG(B33,10)*20</f>
+        <v>19.18082784642187</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>10.1</v>
+      </c>
+      <c r="C34">
+        <f>LOG(B34,10)*20</f>
+        <v>20.086427475652847</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A89103D-81D6-4A69-9C27-66BC04D4E7BA}">
+  <dimension ref="B10:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <f xml:space="preserve"> ('Power Supply'!E6 - 2.6)/0.0005</f>
+        <v>65633.760332114631</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10">
+        <f>'Power Supply'!E6</f>
+        <v>35.416880166057318</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f xml:space="preserve"> ('Power Supply'!E7 - 2.6)/0.0005</f>
+        <v>57025.396744416183</v>
+      </c>
+      <c r="E11">
+        <f>'Power Supply'!E7</f>
+        <v>31.112698372208094</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f xml:space="preserve"> ('Power Supply'!E8 - 2.6)/0.0005</f>
+        <v>58620.985008828276</v>
+      </c>
+      <c r="E12">
+        <f>'Power Supply'!E8</f>
+        <v>31.91049250441414</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D439BB97-2DD2-4CC1-B4D7-155B693D6619}">
+  <dimension ref="B3:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added resistors to library
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A5A219-12A2-477D-8CD1-EEBB0DF41AEF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B3AE02-0545-4B4D-898C-44A9766D8719}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Gain" sheetId="3" r:id="rId3"/>
     <sheet name="Mute Attenuation" sheetId="4" r:id="rId4"/>
     <sheet name="Optional Components" sheetId="5" r:id="rId5"/>
+    <sheet name="Plots" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
   <si>
     <t>http://myhometheater.homestead.com/splcalculator.html</t>
   </si>
@@ -339,9 +340,6 @@
     <t>See 'Gain' sheet</t>
   </si>
   <si>
-    <t>Ci</t>
-  </si>
-  <si>
     <t>Low-frequency roll-off in series with Ri</t>
   </si>
   <si>
@@ -375,6 +373,268 @@
         <family val="2"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>fL = 4hz, Ri = 5750</t>
+  </si>
+  <si>
+    <t>Prevents high-frequency oscillations</t>
+  </si>
+  <si>
+    <t>2.7 (from datasheet)</t>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 1/(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>πR</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 4.8k, R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 2.7</t>
+    </r>
+  </si>
+  <si>
+    <t>Rf1</t>
+  </si>
+  <si>
+    <t>Determines gain</t>
+  </si>
+  <si>
+    <t>Rf2</t>
+  </si>
+  <si>
+    <t>See 'Plots'</t>
+  </si>
+  <si>
+    <t>Works with Cf2 to provide low AC gain at higher frequencies</t>
+  </si>
+  <si>
+    <t>Cf2</t>
+  </si>
+  <si>
+    <t>Works with Rf2 to provide low AC gain at higher frequencies</t>
+  </si>
+  <si>
+    <t>Output Inductance</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f</t>
     </r>
   </si>
 </sst>
@@ -382,7 +642,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +694,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -443,10 +712,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -456,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -469,6 +747,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -584,6 +874,187 @@
         <a:xfrm>
           <a:off x="571500" y="171450"/>
           <a:ext cx="12047619" cy="1180952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>418000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A410A16D-A62B-402C-81FF-F0F3FF22DF25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190499" y="647700"/>
+          <a:ext cx="7542701" cy="4772025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>64130</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8DD9D6B-D1B2-40CD-8107-8DE98DA461BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="647701"/>
+          <a:ext cx="8429625" cy="5321929"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>177560</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>36450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>49695</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>51858</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88C9CA47-0D04-4F78-A248-B56326F8BEFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="177560" y="6703950"/>
+          <a:ext cx="8452918" cy="4206408"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>440252</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>92064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238457</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>98663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5222E18-2D7C-43D1-ADDA-6CF5D9782F3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="440252" y="11712564"/>
+          <a:ext cx="8312090" cy="4197599"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -860,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD76807-681C-4CA7-A650-2C811CF779EA}">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2182,53 +2653,221 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D439BB97-2DD2-4CC1-B4D7-155B693D6619}">
-  <dimension ref="B3:D5"/>
+  <dimension ref="B2:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="8"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
         <v>58</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="10" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63717F91-15B6-43EE-96A3-0BA77994237F}">
+  <dimension ref="F2:K61"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="34" spans="6:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+    </row>
+    <row r="35" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+    </row>
+    <row r="60" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F60" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+    </row>
+    <row r="61" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F2:K3"/>
+    <mergeCell ref="F34:K35"/>
+    <mergeCell ref="F60:K61"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished prototype PCB design
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92226229-DB1F-4AE5-8472-0F8CAD80496E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C17107B-4075-40EF-88DE-7D648B3989D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
   <si>
     <t>http://myhometheater.homestead.com/splcalculator.html</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>fL = 4.5kHz, Ri = 6340</t>
+  </si>
+  <si>
+    <t>fc = 30k, RSN = 2.7</t>
   </si>
 </sst>
 </file>
@@ -1501,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEB1EA-E152-4802-8ABB-B4D06F75C74E}">
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD76807-681C-4CA7-A650-2C811CF779EA}">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2659,7 +2662,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2749,6 +2752,9 @@
       <c r="E7" s="10" t="s">
         <v>68</v>
       </c>
+      <c r="F7" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -2812,23 +2818,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63717F91-15B6-43EE-96A3-0BA77994237F}">
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -2841,8 +2852,11 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="P2" s="7"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -2851,43 +2865,43 @@
       <c r="K3" s="12"/>
       <c r="P3" s="7"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P4" s="7"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P6" s="7"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P7" s="7"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P8" s="7"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P10" s="7"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P11" s="7"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P12" s="7"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P13" s="7"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P16" s="7"/>
     </row>
     <row r="17" spans="16:16" x14ac:dyDescent="0.25">
@@ -3126,11 +3140,12 @@
       <c r="P85" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="F2:K3"/>
     <mergeCell ref="F34:K35"/>
     <mergeCell ref="F60:K61"/>
     <mergeCell ref="A1:C2"/>
+    <mergeCell ref="Q1:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added spreadsheet for test cases
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89154013-64E7-45BB-BEF6-5122EA90E0F3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05547888-A9C8-4766-8D01-3105C537733C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2172,7 +2172,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2899,7 +2899,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added folder for simulation results
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05547888-A9C8-4766-8D01-3105C537733C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DC1727-9DB8-49D1-A8DA-D304A7669596}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9510" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="4665" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,16 @@
     <sheet name="Plots" sheetId="7" r:id="rId6"/>
     <sheet name="Heat Sinking" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -896,13 +902,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1571,25 +1577,25 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" customWidth="1"/>
+    <col min="3" max="3" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1606,7 +1612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>88.3</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>93.4</v>
       </c>
@@ -1660,12 +1666,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>90</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>88.3</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>105.3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1734,30 +1740,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEB1EA-E152-4802-8ABB-B4D06F75C74E}">
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" customWidth="1"/>
+    <col min="4" max="4" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.86328125" customWidth="1"/>
+    <col min="11" max="11" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>25</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>26</v>
       </c>
@@ -1779,7 +1785,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>115</v>
       </c>
@@ -1795,7 +1801,7 @@
         <v>33.941125496954285</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="15.75" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
         <v>120</v>
       </c>
@@ -1814,50 +1820,51 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>117</v>
       </c>
       <c r="C7">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <f>POWER((B7/C7), 2)</f>
-        <v>28.283057851239672</v>
+        <v>23.765625</v>
       </c>
       <c r="E7">
         <f>C7*SQRT(2)</f>
-        <v>31.112698372208094</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+        <v>33.941125496954285</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>120</v>
       </c>
       <c r="C8">
         <f>B8/SQRT(D8)</f>
-        <v>22.564125640873733</v>
+        <v>24.615384615384617</v>
       </c>
       <c r="D8">
-        <v>28.283000000000001</v>
+        <f>D7</f>
+        <v>23.765625</v>
       </c>
       <c r="E8">
         <f>C8*SQRT(2)</f>
-        <v>31.91049250441414</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+        <v>34.81141076610696</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="11"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="12"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>13</v>
       </c>
@@ -1883,7 +1890,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C17">
         <v>4</v>
       </c>
@@ -1913,7 +1920,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C18">
         <v>4</v>
       </c>
@@ -1943,7 +1950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C19">
         <v>4</v>
       </c>
@@ -1973,12 +1980,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>13</v>
       </c>
@@ -2000,7 +2007,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C23">
         <v>4</v>
       </c>
@@ -2026,7 +2033,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C24">
         <v>4</v>
       </c>
@@ -2052,7 +2059,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C25">
         <v>4</v>
       </c>
@@ -2076,7 +2083,7 @@
         <v>17.868763676314927</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C26">
         <v>5</v>
       </c>
@@ -2100,7 +2107,7 @@
         <v>19.977885127059611</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" ht="16.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
         <v>34</v>
       </c>
@@ -2108,7 +2115,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B30">
         <f>E6</f>
         <v>35.416880166057318</v>
@@ -2118,27 +2125,27 @@
         <v>63.546386953382587</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B31">
         <f t="shared" ref="B31:B32" si="0">E7</f>
-        <v>31.112698372208094</v>
+        <v>33.941125496954285</v>
       </c>
       <c r="C31">
         <f>POWER(2*E7,2)/(2*POWER(PI(),2)*$C$24)</f>
-        <v>49.039452882891489</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+        <v>58.361001777986573</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>31.91049250441414</v>
+        <v>34.81141076610696</v>
       </c>
       <c r="C32">
         <f>POWER(2*E8,2)/(2*POWER(PI(),2)*$C$24)</f>
-        <v>51.586643724133381</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+        <v>61.392243816422429</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>49</v>
       </c>
@@ -2146,7 +2153,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35">
         <f>C30*4 + (Gain!H10*2) + (Gain!H19*2)</f>
         <v>564.5855478135303</v>
@@ -2175,19 +2182,19 @@
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>43</v>
       </c>
@@ -2201,7 +2208,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -2227,7 +2234,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>16</v>
       </c>
@@ -2258,7 +2265,7 @@
         <v>3.9959028968642611</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B7">
         <f>B6+0.2</f>
         <v>16.2</v>
@@ -2290,7 +2297,7 @@
         <v>4.0511969297674684</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B8">
         <f t="shared" ref="B8:B10" si="5">B7+0.2</f>
         <v>16.399999999999999</v>
@@ -2322,7 +2329,7 @@
         <v>4.0969523072024012</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B9">
         <f t="shared" si="5"/>
         <v>16.599999999999998</v>
@@ -2354,7 +2361,7 @@
         <v>4.1474764014059335</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2389,7 +2396,7 @@
         <v>4.1997857306837361</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>17</v>
       </c>
@@ -2420,7 +2427,7 @@
         <v>4.249111714234969</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>17.5</v>
       </c>
@@ -2451,7 +2458,7 @@
         <v>4.3746873051096591</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B13">
         <f>B12+0.1</f>
         <v>17.600000000000001</v>
@@ -2483,7 +2490,7 @@
         <v>4.4012281404561397</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B14">
         <f t="shared" ref="B14:B16" si="8">B13+0.1</f>
         <v>17.700000000000003</v>
@@ -2509,7 +2516,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B15">
         <f t="shared" si="8"/>
         <v>17.800000000000004</v>
@@ -2541,7 +2548,7 @@
         <v>4.4465165898760093</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B16">
         <f t="shared" si="8"/>
         <v>17.900000000000006</v>
@@ -2567,7 +2574,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>18</v>
       </c>
@@ -2598,7 +2605,7 @@
         <v>4.500376387410375</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B18">
         <f>B17+0.2</f>
         <v>18.2</v>
@@ -2624,7 +2631,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2659,7 +2666,7 @@
         <v>4.6002704042758937</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B20">
         <f t="shared" si="12"/>
         <v>18.599999999999998</v>
@@ -2685,7 +2692,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B21">
         <f t="shared" si="12"/>
         <v>18.799999999999997</v>
@@ -2711,7 +2718,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>19</v>
       </c>
@@ -2742,7 +2749,7 @@
         <v>4.7507256043531036</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>1.1000000000000001</v>
       </c>
@@ -2751,7 +2758,7 @@
         <v>0.82785370316450146</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>2.1</v>
       </c>
@@ -2760,7 +2767,7 @@
         <v>6.4443858946783852</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B27">
         <v>3.1</v>
       </c>
@@ -2772,7 +2779,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>4.0999999999999996</v>
       </c>
@@ -2781,7 +2788,7 @@
         <v>12.255677134394709</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>5.0999999999999996</v>
       </c>
@@ -2790,7 +2797,7 @@
         <v>14.151403521958725</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>6.1</v>
       </c>
@@ -2799,7 +2806,7 @@
         <v>15.706596700215339</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>7.1</v>
       </c>
@@ -2808,7 +2815,7 @@
         <v>17.025166974381506</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>8.1</v>
       </c>
@@ -2817,7 +2824,7 @@
         <v>18.169700377572994</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>9.1</v>
       </c>
@@ -2826,7 +2833,7 @@
         <v>19.18082784642187</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34">
         <v>10.1</v>
       </c>
@@ -2849,9 +2856,9 @@
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5" t="s">
         <v>50</v>
       </c>
@@ -2867,24 +2874,24 @@
         <v>35.416880166057318</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C11">
         <f xml:space="preserve"> ('Power Supply'!E7 - 2.6)/0.0005</f>
-        <v>57025.396744416183</v>
+        <v>62682.250993908565</v>
       </c>
       <c r="E11">
         <f>'Power Supply'!E7</f>
-        <v>31.112698372208094</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+        <v>33.941125496954285</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C12">
         <f xml:space="preserve"> ('Power Supply'!E8 - 2.6)/0.0005</f>
-        <v>58620.985008828276</v>
+        <v>64422.821532213915</v>
       </c>
       <c r="E12">
         <f>'Power Supply'!E8</f>
-        <v>31.91049250441414</v>
+        <v>34.81141076610696</v>
       </c>
     </row>
   </sheetData>
@@ -2898,23 +2905,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D439BB97-2DD2-4CC1-B4D7-155B693D6619}">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="57.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.73046875" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>53</v>
       </c>
@@ -2931,7 +2938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>67</v>
       </c>
@@ -2948,7 +2955,7 @@
         <v>6340</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>66</v>
       </c>
@@ -2965,7 +2972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>64</v>
       </c>
@@ -2976,7 +2983,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
         <v>65</v>
       </c>
@@ -2993,7 +3000,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>69</v>
       </c>
@@ -3004,7 +3011,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>71</v>
       </c>
@@ -3015,7 +3022,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>74</v>
       </c>
@@ -3026,25 +3033,25 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D17" s="7"/>
     </row>
   </sheetData>
@@ -3061,319 +3068,319 @@
       <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="P1" s="7"/>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="F2" s="12" t="s">
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="F2" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
       <c r="P2" s="7"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
       <c r="P3" s="7"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P4" s="7"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P6" s="7"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P7" s="7"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P8" s="7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P11" s="7"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P12" s="7"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P13" s="7"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="P16" s="7"/>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P17" s="7"/>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P18" s="7"/>
     </row>
-    <row r="19" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P19" s="7"/>
     </row>
-    <row r="20" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P20" s="7"/>
     </row>
-    <row r="21" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P21" s="7"/>
     </row>
-    <row r="22" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P22" s="7"/>
     </row>
-    <row r="23" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P25" s="7"/>
     </row>
-    <row r="26" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P26" s="7"/>
     </row>
-    <row r="27" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P27" s="7"/>
     </row>
-    <row r="28" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P28" s="7"/>
     </row>
-    <row r="29" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P29" s="7"/>
     </row>
-    <row r="30" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P30" s="7"/>
     </row>
-    <row r="31" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P31" s="7"/>
     </row>
-    <row r="32" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P32" s="7"/>
     </row>
-    <row r="33" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P33" s="7"/>
     </row>
-    <row r="34" spans="6:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F34" s="12" t="s">
+    <row r="34" spans="6:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F34" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
       <c r="P34" s="7"/>
     </row>
-    <row r="35" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
+    <row r="35" spans="6:16" x14ac:dyDescent="0.45">
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
       <c r="P35" s="7"/>
     </row>
-    <row r="36" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P36" s="7"/>
     </row>
-    <row r="37" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P37" s="7"/>
     </row>
-    <row r="38" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P38" s="7"/>
     </row>
-    <row r="39" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P39" s="7"/>
     </row>
-    <row r="40" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P40" s="7"/>
     </row>
-    <row r="41" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P41" s="7"/>
     </row>
-    <row r="42" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P42" s="7"/>
     </row>
-    <row r="43" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P43" s="7"/>
     </row>
-    <row r="44" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P44" s="7"/>
     </row>
-    <row r="45" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P45" s="7"/>
     </row>
-    <row r="46" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P46" s="7"/>
     </row>
-    <row r="47" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P47" s="7"/>
     </row>
-    <row r="48" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P48" s="7"/>
     </row>
-    <row r="49" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P49" s="7"/>
     </row>
-    <row r="50" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P50" s="7"/>
     </row>
-    <row r="51" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P51" s="7"/>
     </row>
-    <row r="52" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P52" s="7"/>
     </row>
-    <row r="53" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P53" s="7"/>
     </row>
-    <row r="54" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P54" s="7"/>
     </row>
-    <row r="55" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P55" s="7"/>
     </row>
-    <row r="56" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P56" s="7"/>
     </row>
-    <row r="57" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P57" s="7"/>
     </row>
-    <row r="58" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P58" s="7"/>
     </row>
-    <row r="59" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P59" s="7"/>
     </row>
-    <row r="60" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F60" s="12" t="s">
+    <row r="60" spans="6:16" x14ac:dyDescent="0.45">
+      <c r="F60" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
-      <c r="K60" s="12"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
       <c r="P60" s="7"/>
     </row>
-    <row r="61" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-      <c r="K61" s="12"/>
+    <row r="61" spans="6:16" x14ac:dyDescent="0.45">
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
       <c r="P61" s="7"/>
     </row>
-    <row r="62" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P62" s="7"/>
     </row>
-    <row r="63" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P63" s="7"/>
     </row>
-    <row r="64" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:16" x14ac:dyDescent="0.45">
       <c r="P64" s="7"/>
     </row>
-    <row r="65" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P65" s="7"/>
     </row>
-    <row r="66" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P66" s="7"/>
     </row>
-    <row r="67" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P67" s="7"/>
     </row>
-    <row r="68" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P68" s="7"/>
     </row>
-    <row r="69" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P69" s="7"/>
     </row>
-    <row r="70" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P70" s="7"/>
     </row>
-    <row r="71" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P71" s="7"/>
     </row>
-    <row r="72" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P72" s="7"/>
     </row>
-    <row r="73" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P73" s="7"/>
     </row>
-    <row r="74" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P74" s="7"/>
     </row>
-    <row r="75" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P75" s="7"/>
     </row>
-    <row r="76" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P76" s="7"/>
     </row>
-    <row r="77" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P77" s="7"/>
     </row>
-    <row r="78" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P78" s="7"/>
     </row>
-    <row r="79" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P79" s="7"/>
     </row>
-    <row r="80" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P80" s="7"/>
     </row>
-    <row r="81" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P81" s="7"/>
     </row>
-    <row r="82" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P82" s="7"/>
     </row>
-    <row r="83" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P83" s="7"/>
     </row>
-    <row r="84" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P84" s="7"/>
     </row>
-    <row r="85" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P85" s="7"/>
     </row>
   </sheetData>
@@ -3398,17 +3405,17 @@
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>81</v>
       </c>
@@ -3417,8 +3424,8 @@
         <v>63.546386953382587</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C5">
@@ -3428,8 +3435,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="11" t="s">
         <v>85</v>
       </c>
       <c r="C6">
@@ -3439,8 +3446,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="11" t="s">
         <v>84</v>
       </c>
       <c r="C7">
@@ -3450,16 +3457,16 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="11" t="s">
         <v>86</v>
       </c>
       <c r="C8">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="11" t="s">
         <v>87</v>
       </c>
       <c r="C9">
@@ -3470,12 +3477,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>81</v>
       </c>
@@ -3484,24 +3491,24 @@
         <v>127.09277390676517</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B14" s="13" t="s">
+    <row r="14" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="11" t="s">
         <v>85</v>
       </c>
       <c r="C15">
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="11" t="s">
         <v>93</v>
       </c>
       <c r="C16">
@@ -3512,8 +3519,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="11" t="s">
         <v>94</v>
       </c>
       <c r="C17">
@@ -3524,24 +3531,24 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B18" s="13" t="s">
+    <row r="18" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="11" t="s">
         <v>84</v>
       </c>
       <c r="C18">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="11" t="s">
         <v>86</v>
       </c>
       <c r="C19">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="11" t="s">
         <v>87</v>
       </c>
       <c r="C20">

</xml_diff>

<commit_message>
Added total ideal sim and stability sim
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DC1727-9DB8-49D1-A8DA-D304A7669596}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E6E611-1066-4E1A-A10D-7F1838274A52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="4665" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="4665" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
     <sheet name="Power Supply" sheetId="2" r:id="rId2"/>
     <sheet name="Gain" sheetId="3" r:id="rId3"/>
-    <sheet name="Mute Attenuation" sheetId="4" r:id="rId4"/>
-    <sheet name="Optional Components" sheetId="5" r:id="rId5"/>
-    <sheet name="Plots" sheetId="7" r:id="rId6"/>
-    <sheet name="Heat Sinking" sheetId="8" r:id="rId7"/>
+    <sheet name="Power Resistors" sheetId="9" r:id="rId4"/>
+    <sheet name="Mute Attenuation" sheetId="4" r:id="rId5"/>
+    <sheet name="Optional Components" sheetId="5" r:id="rId6"/>
+    <sheet name="Plots" sheetId="7" r:id="rId7"/>
+    <sheet name="Heat Sinking" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
   <si>
     <t>http://myhometheater.homestead.com/splcalculator.html</t>
   </si>
@@ -784,6 +785,30 @@
   </si>
   <si>
     <t>Total Current (Max)</t>
+  </si>
+  <si>
+    <t>Voltage Output (Max)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req </t>
+  </si>
+  <si>
+    <t># of Resistors</t>
+  </si>
+  <si>
+    <t>Load Current (Max)</t>
+  </si>
+  <si>
+    <t>Nominal Resistance</t>
+  </si>
+  <si>
+    <t>RMS Power Dissipated (Per Resistor)</t>
+  </si>
+  <si>
+    <t>Cost Per Resistor</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
   </si>
 </sst>
 </file>
@@ -1740,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEB1EA-E152-4802-8ABB-B4D06F75C74E}">
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2179,7 +2204,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2199,7 +2224,7 @@
         <v>43</v>
       </c>
       <c r="D3">
-        <v>100000</v>
+        <v>20000</v>
       </c>
       <c r="F3" t="s">
         <v>46</v>
@@ -2244,7 +2269,7 @@
       </c>
       <c r="D6">
         <f>$D$3/(B6-1)</f>
-        <v>6666.666666666667</v>
+        <v>1333.3333333333333</v>
       </c>
       <c r="E6">
         <v>11.32</v>
@@ -2276,7 +2301,7 @@
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D10" si="2">$D$3/(B7-1)</f>
-        <v>6578.9473684210525</v>
+        <v>1315.7894736842106</v>
       </c>
       <c r="E7">
         <v>11.45</v>
@@ -2308,7 +2333,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>6493.5064935064938</v>
+        <v>1298.7012987012988</v>
       </c>
       <c r="E8">
         <v>11.6</v>
@@ -2340,7 +2365,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>6410.2564102564111</v>
+        <v>1282.0512820512822</v>
       </c>
       <c r="E9">
         <v>11.74</v>
@@ -2375,7 +2400,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>6329.1139240506336</v>
+        <v>1265.8227848101269</v>
       </c>
       <c r="E10">
         <v>11.88</v>
@@ -2406,7 +2431,7 @@
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D16" si="6">$D$3/(B11-1)</f>
-        <v>6250</v>
+        <v>1250</v>
       </c>
       <c r="E11">
         <v>12.02</v>
@@ -2437,7 +2462,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="6"/>
-        <v>6060.606060606061</v>
+        <v>1212.121212121212</v>
       </c>
       <c r="E12">
         <v>12.37</v>
@@ -2469,7 +2494,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="6"/>
-        <v>6024.0963855421678</v>
+        <v>1204.8192771084337</v>
       </c>
       <c r="E13">
         <v>12.44</v>
@@ -2501,7 +2526,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="6"/>
-        <v>5988.0239520958075</v>
+        <v>1197.6047904191614</v>
       </c>
       <c r="F14">
         <f t="shared" si="7"/>
@@ -2527,7 +2552,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="6"/>
-        <v>5952.3809523809505</v>
+        <v>1190.4761904761901</v>
       </c>
       <c r="E15">
         <v>12.59</v>
@@ -2559,7 +2584,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="6"/>
-        <v>5917.1597633136071</v>
+        <v>1183.4319526627214</v>
       </c>
       <c r="F16">
         <f t="shared" si="7"/>
@@ -2584,7 +2609,7 @@
       </c>
       <c r="D17">
         <f>$D$3/(B17-1)</f>
-        <v>5882.3529411764703</v>
+        <v>1176.4705882352941</v>
       </c>
       <c r="E17">
         <v>12.73</v>
@@ -2616,7 +2641,7 @@
       </c>
       <c r="D18">
         <f t="shared" ref="D18:D21" si="10">$D$3/(B18-1)</f>
-        <v>5813.9534883720935</v>
+        <v>1162.7906976744187</v>
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F21" si="11">E18*SQRT(2)</f>
@@ -2645,7 +2670,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="10"/>
-        <v>5747.1264367816093</v>
+        <v>1149.4252873563219</v>
       </c>
       <c r="E19">
         <v>13.01</v>
@@ -2677,7 +2702,7 @@
       </c>
       <c r="D20">
         <f t="shared" si="10"/>
-        <v>5681.8181818181829</v>
+        <v>1136.3636363636365</v>
       </c>
       <c r="F20">
         <f t="shared" si="11"/>
@@ -2703,7 +2728,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="10"/>
-        <v>5617.9775280898884</v>
+        <v>1123.5955056179778</v>
       </c>
       <c r="F21">
         <f t="shared" si="11"/>
@@ -2728,7 +2753,7 @@
       </c>
       <c r="D22">
         <f>$D$3/(B22-1)</f>
-        <v>5555.5555555555557</v>
+        <v>1111.1111111111111</v>
       </c>
       <c r="E22">
         <v>13.43</v>
@@ -2849,6 +2874,195 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303E5587-B5A3-4B05-AB52-57C1D2A24CD5}">
+  <dimension ref="B2:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="E2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2">
+        <f>C2/F2</f>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f>(POWER($I$2/C5,2)*B5)/SQRT(2)</f>
+        <v>59.849517959629367</v>
+      </c>
+      <c r="E5">
+        <v>17.97</v>
+      </c>
+      <c r="F5">
+        <f>E5*C5</f>
+        <v>17.97</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <f>B5*2</f>
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D11" si="0">(POWER($I$2/C6,2)*B6)/SQRT(2)</f>
+        <v>29.924758979814683</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F11" si="1">E6*C6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <f t="shared" ref="B7:B11" si="2">B6*2</f>
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <f>C6*C6</f>
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>14.962379489907342</v>
+      </c>
+      <c r="E7">
+        <v>2.93</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>11.72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:C11" si="3">C7*C7</f>
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.8702974362384177</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.4611698720612638E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="3"/>
+        <v>65536</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>4.4591365724525874E-7</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="3"/>
+        <v>4294967296</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.076447276609292E-16</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A89103D-81D6-4A69-9C27-66BC04D4E7BA}">
   <dimension ref="B10:E12"/>
   <sheetViews>
@@ -2901,7 +3115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D439BB97-2DD2-4CC1-B4D7-155B693D6619}">
   <dimension ref="B2:F17"/>
   <sheetViews>
@@ -3060,7 +3274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63717F91-15B6-43EE-96A3-0BA77994237F}">
   <dimension ref="A1:S85"/>
   <sheetViews>
@@ -3397,7 +3611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFCE619-66E5-4E0A-A1ED-041ECE06AB55}">
   <dimension ref="B2:D20"/>
   <sheetViews>

</xml_diff>

<commit_message>
fixed old transformer sim
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E6E611-1066-4E1A-A10D-7F1838274A52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC4D333-A6D6-4AC9-82F9-2C00D9CEC1DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="4665" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
@@ -1765,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEB1EA-E152-4802-8ABB-B4D06F75C74E}">
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2204,7 +2204,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2224,7 +2224,7 @@
         <v>43</v>
       </c>
       <c r="D3">
-        <v>20000</v>
+        <v>100000</v>
       </c>
       <c r="F3" t="s">
         <v>46</v>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="D6">
         <f>$D$3/(B6-1)</f>
-        <v>1333.3333333333333</v>
+        <v>6666.666666666667</v>
       </c>
       <c r="E6">
         <v>11.32</v>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D10" si="2">$D$3/(B7-1)</f>
-        <v>1315.7894736842106</v>
+        <v>6578.9473684210525</v>
       </c>
       <c r="E7">
         <v>11.45</v>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>1298.7012987012988</v>
+        <v>6493.5064935064938</v>
       </c>
       <c r="E8">
         <v>11.6</v>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>1282.0512820512822</v>
+        <v>6410.2564102564111</v>
       </c>
       <c r="E9">
         <v>11.74</v>
@@ -2400,7 +2400,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>1265.8227848101269</v>
+        <v>6329.1139240506336</v>
       </c>
       <c r="E10">
         <v>11.88</v>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D16" si="6">$D$3/(B11-1)</f>
-        <v>1250</v>
+        <v>6250</v>
       </c>
       <c r="E11">
         <v>12.02</v>
@@ -2462,7 +2462,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="6"/>
-        <v>1212.121212121212</v>
+        <v>6060.606060606061</v>
       </c>
       <c r="E12">
         <v>12.37</v>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="6"/>
-        <v>1204.8192771084337</v>
+        <v>6024.0963855421678</v>
       </c>
       <c r="E13">
         <v>12.44</v>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="6"/>
-        <v>1197.6047904191614</v>
+        <v>5988.0239520958075</v>
       </c>
       <c r="F14">
         <f t="shared" si="7"/>
@@ -2552,7 +2552,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="6"/>
-        <v>1190.4761904761901</v>
+        <v>5952.3809523809505</v>
       </c>
       <c r="E15">
         <v>12.59</v>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="6"/>
-        <v>1183.4319526627214</v>
+        <v>5917.1597633136071</v>
       </c>
       <c r="F16">
         <f t="shared" si="7"/>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="D17">
         <f>$D$3/(B17-1)</f>
-        <v>1176.4705882352941</v>
+        <v>5882.3529411764703</v>
       </c>
       <c r="E17">
         <v>12.73</v>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="D18">
         <f t="shared" ref="D18:D21" si="10">$D$3/(B18-1)</f>
-        <v>1162.7906976744187</v>
+        <v>5813.9534883720935</v>
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F21" si="11">E18*SQRT(2)</f>
@@ -2670,7 +2670,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="10"/>
-        <v>1149.4252873563219</v>
+        <v>5747.1264367816093</v>
       </c>
       <c r="E19">
         <v>13.01</v>
@@ -2702,7 +2702,7 @@
       </c>
       <c r="D20">
         <f t="shared" si="10"/>
-        <v>1136.3636363636365</v>
+        <v>5681.8181818181829</v>
       </c>
       <c r="F20">
         <f t="shared" si="11"/>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="10"/>
-        <v>1123.5955056179778</v>
+        <v>5617.9775280898884</v>
       </c>
       <c r="F21">
         <f t="shared" si="11"/>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="D22">
         <f>$D$3/(B22-1)</f>
-        <v>1111.1111111111111</v>
+        <v>5555.5555555555557</v>
       </c>
       <c r="E22">
         <v>13.43</v>
@@ -2877,8 +2877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303E5587-B5A3-4B05-AB52-57C1D2A24CD5}">
   <dimension ref="B2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
added kicad project for amplifier board
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC4D333-A6D6-4AC9-82F9-2C00D9CEC1DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7658050F-A4EB-5247-9040-D518BE756E95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1602,25 +1604,25 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.73046875" customWidth="1"/>
-    <col min="3" max="3" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1637,7 +1639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>88.3</v>
       </c>
@@ -1674,7 +1676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>93.4</v>
       </c>
@@ -1691,12 +1693,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>90</v>
       </c>
@@ -1713,7 +1715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>88.3</v>
       </c>
@@ -1727,7 +1729,7 @@
         <v>105.3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1769,26 +1771,26 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.86328125" customWidth="1"/>
-    <col min="11" max="11" width="14.59765625" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>25</v>
       </c>
@@ -1796,7 +1798,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>26</v>
       </c>
@@ -1810,7 +1812,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>115</v>
       </c>
@@ -1826,7 +1828,7 @@
         <v>33.941125496954285</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:11" ht="17" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>120</v>
       </c>
@@ -1845,7 +1847,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>117</v>
       </c>
@@ -1861,7 +1863,7 @@
         <v>33.941125496954285</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>120</v>
       </c>
@@ -1878,18 +1880,18 @@
         <v>34.81141076610696</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="12"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>13</v>
       </c>
@@ -1915,7 +1917,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C17">
         <v>4</v>
       </c>
@@ -1945,7 +1947,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>4</v>
       </c>
@@ -1975,7 +1977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>4</v>
       </c>
@@ -2005,12 +2007,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>13</v>
       </c>
@@ -2032,7 +2034,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C23">
         <v>4</v>
       </c>
@@ -2058,7 +2060,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C24">
         <v>4</v>
       </c>
@@ -2084,7 +2086,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C25">
         <v>4</v>
       </c>
@@ -2108,7 +2110,7 @@
         <v>17.868763676314927</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C26">
         <v>5</v>
       </c>
@@ -2132,7 +2134,7 @@
         <v>19.977885127059611</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="16.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>34</v>
       </c>
@@ -2140,7 +2142,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30">
         <f>E6</f>
         <v>35.416880166057318</v>
@@ -2150,7 +2152,7 @@
         <v>63.546386953382587</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31">
         <f t="shared" ref="B31:B32" si="0">E7</f>
         <v>33.941125496954285</v>
@@ -2160,7 +2162,7 @@
         <v>58.361001777986573</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32">
         <f t="shared" si="0"/>
         <v>34.81141076610696</v>
@@ -2170,7 +2172,7 @@
         <v>61.392243816422429</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>49</v>
       </c>
@@ -2178,7 +2180,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35">
         <f>C30*4 + (Gain!H10*2) + (Gain!H19*2)</f>
         <v>564.5855478135303</v>
@@ -2207,19 +2209,19 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>43</v>
       </c>
@@ -2233,7 +2235,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -2259,7 +2261,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>16</v>
       </c>
@@ -2290,7 +2292,7 @@
         <v>3.9959028968642611</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <f>B6+0.2</f>
         <v>16.2</v>
@@ -2322,7 +2324,7 @@
         <v>4.0511969297674684</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" ref="B8:B10" si="5">B7+0.2</f>
         <v>16.399999999999999</v>
@@ -2354,7 +2356,7 @@
         <v>4.0969523072024012</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="5"/>
         <v>16.599999999999998</v>
@@ -2386,7 +2388,7 @@
         <v>4.1474764014059335</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2421,7 +2423,7 @@
         <v>4.1997857306837361</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>17</v>
       </c>
@@ -2452,7 +2454,7 @@
         <v>4.249111714234969</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>17.5</v>
       </c>
@@ -2483,7 +2485,7 @@
         <v>4.3746873051096591</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13">
         <f>B12+0.1</f>
         <v>17.600000000000001</v>
@@ -2515,7 +2517,7 @@
         <v>4.4012281404561397</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14">
         <f t="shared" ref="B14:B16" si="8">B13+0.1</f>
         <v>17.700000000000003</v>
@@ -2541,7 +2543,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15">
         <f t="shared" si="8"/>
         <v>17.800000000000004</v>
@@ -2573,7 +2575,7 @@
         <v>4.4465165898760093</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16">
         <f t="shared" si="8"/>
         <v>17.900000000000006</v>
@@ -2599,7 +2601,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>18</v>
       </c>
@@ -2630,7 +2632,7 @@
         <v>4.500376387410375</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B18">
         <f>B17+0.2</f>
         <v>18.2</v>
@@ -2656,7 +2658,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2691,7 +2693,7 @@
         <v>4.6002704042758937</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B20">
         <f t="shared" si="12"/>
         <v>18.599999999999998</v>
@@ -2717,7 +2719,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B21">
         <f t="shared" si="12"/>
         <v>18.799999999999997</v>
@@ -2743,7 +2745,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>19</v>
       </c>
@@ -2774,7 +2776,7 @@
         <v>4.7507256043531036</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>1.1000000000000001</v>
       </c>
@@ -2783,7 +2785,7 @@
         <v>0.82785370316450146</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>2.1</v>
       </c>
@@ -2792,7 +2794,7 @@
         <v>6.4443858946783852</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>3.1</v>
       </c>
@@ -2804,7 +2806,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>4.0999999999999996</v>
       </c>
@@ -2813,7 +2815,7 @@
         <v>12.255677134394709</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>5.0999999999999996</v>
       </c>
@@ -2822,7 +2824,7 @@
         <v>14.151403521958725</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>6.1</v>
       </c>
@@ -2831,7 +2833,7 @@
         <v>15.706596700215339</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>7.1</v>
       </c>
@@ -2840,7 +2842,7 @@
         <v>17.025166974381506</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>8.1</v>
       </c>
@@ -2849,7 +2851,7 @@
         <v>18.169700377572994</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>9.1</v>
       </c>
@@ -2858,7 +2860,7 @@
         <v>19.18082784642187</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>10.1</v>
       </c>
@@ -2881,16 +2883,16 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>98</v>
       </c>
@@ -2911,7 +2913,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>102</v>
       </c>
@@ -2928,7 +2930,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>4</v>
       </c>
@@ -2947,7 +2949,7 @@
         <v>17.97</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <f>B5*2</f>
         <v>8</v>
@@ -2964,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <f t="shared" ref="B7:B11" si="2">B6*2</f>
         <v>16</v>
@@ -2985,7 +2987,7 @@
         <v>11.72</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -3003,7 +3005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="2"/>
         <v>64</v>
@@ -3021,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" si="2"/>
         <v>128</v>
@@ -3039,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11">
         <f t="shared" si="2"/>
         <v>256</v>
@@ -3070,9 +3072,9 @@
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>50</v>
       </c>
@@ -3088,7 +3090,7 @@
         <v>35.416880166057318</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C11">
         <f xml:space="preserve"> ('Power Supply'!E7 - 2.6)/0.0005</f>
         <v>62682.250993908565</v>
@@ -3098,7 +3100,7 @@
         <v>33.941125496954285</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C12">
         <f xml:space="preserve"> ('Power Supply'!E8 - 2.6)/0.0005</f>
         <v>64422.821532213915</v>
@@ -3123,19 +3125,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="57.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.73046875" customWidth="1"/>
-    <col min="6" max="6" width="19.265625" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>53</v>
       </c>
@@ -3152,7 +3154,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>67</v>
       </c>
@@ -3169,7 +3171,7 @@
         <v>6340</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>66</v>
       </c>
@@ -3186,7 +3188,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>64</v>
       </c>
@@ -3197,7 +3199,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>65</v>
       </c>
@@ -3214,7 +3216,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>69</v>
       </c>
@@ -3225,7 +3227,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>71</v>
       </c>
@@ -3236,7 +3238,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>74</v>
       </c>
@@ -3247,25 +3249,25 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" s="7"/>
     </row>
   </sheetData>
@@ -3282,9 +3284,9 @@
       <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>20</v>
       </c>
@@ -3297,7 +3299,7 @@
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -3314,7 +3316,7 @@
       <c r="R2" s="13"/>
       <c r="S2" s="13"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -3323,97 +3325,97 @@
       <c r="K3" s="13"/>
       <c r="P3" s="7"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P4" s="7"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P6" s="7"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P7" s="7"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P8" s="7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P11" s="7"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P12" s="7"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P13" s="7"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P16" s="7"/>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P17" s="7"/>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="18" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P18" s="7"/>
     </row>
-    <row r="19" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="19" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P19" s="7"/>
     </row>
-    <row r="20" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P20" s="7"/>
     </row>
-    <row r="21" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="21" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P21" s="7"/>
     </row>
-    <row r="22" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="22" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P22" s="7"/>
     </row>
-    <row r="23" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="23" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="24" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="25" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P25" s="7"/>
     </row>
-    <row r="26" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="26" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P26" s="7"/>
     </row>
-    <row r="27" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="27" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P27" s="7"/>
     </row>
-    <row r="28" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="28" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P28" s="7"/>
     </row>
-    <row r="29" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="29" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P29" s="7"/>
     </row>
-    <row r="30" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="30" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P30" s="7"/>
     </row>
-    <row r="31" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="31" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P31" s="7"/>
     </row>
-    <row r="32" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="32" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P32" s="7"/>
     </row>
-    <row r="33" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="33" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P33" s="7"/>
     </row>
-    <row r="34" spans="6:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="6:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F34" s="13" t="s">
         <v>77</v>
       </c>
@@ -3424,7 +3426,7 @@
       <c r="K34" s="13"/>
       <c r="P34" s="7"/>
     </row>
-    <row r="35" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="35" spans="6:16" x14ac:dyDescent="0.2">
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -3433,79 +3435,79 @@
       <c r="K35" s="13"/>
       <c r="P35" s="7"/>
     </row>
-    <row r="36" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="36" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P36" s="7"/>
     </row>
-    <row r="37" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P37" s="7"/>
     </row>
-    <row r="38" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="38" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P38" s="7"/>
     </row>
-    <row r="39" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P39" s="7"/>
     </row>
-    <row r="40" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P40" s="7"/>
     </row>
-    <row r="41" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="41" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P41" s="7"/>
     </row>
-    <row r="42" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="42" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P42" s="7"/>
     </row>
-    <row r="43" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="43" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P43" s="7"/>
     </row>
-    <row r="44" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="44" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P44" s="7"/>
     </row>
-    <row r="45" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="45" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P45" s="7"/>
     </row>
-    <row r="46" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="46" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P46" s="7"/>
     </row>
-    <row r="47" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="47" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P47" s="7"/>
     </row>
-    <row r="48" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="48" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P48" s="7"/>
     </row>
-    <row r="49" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="49" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P49" s="7"/>
     </row>
-    <row r="50" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="50" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P50" s="7"/>
     </row>
-    <row r="51" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="51" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P51" s="7"/>
     </row>
-    <row r="52" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="52" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P52" s="7"/>
     </row>
-    <row r="53" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="53" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P53" s="7"/>
     </row>
-    <row r="54" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="54" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P54" s="7"/>
     </row>
-    <row r="55" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="55" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P55" s="7"/>
     </row>
-    <row r="56" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="56" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P56" s="7"/>
     </row>
-    <row r="57" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="57" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P57" s="7"/>
     </row>
-    <row r="58" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="58" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P58" s="7"/>
     </row>
-    <row r="59" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="59" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P59" s="7"/>
     </row>
-    <row r="60" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="60" spans="6:16" x14ac:dyDescent="0.2">
       <c r="F60" s="13" t="s">
         <v>76</v>
       </c>
@@ -3516,7 +3518,7 @@
       <c r="K60" s="13"/>
       <c r="P60" s="7"/>
     </row>
-    <row r="61" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="61" spans="6:16" x14ac:dyDescent="0.2">
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
@@ -3525,76 +3527,76 @@
       <c r="K61" s="13"/>
       <c r="P61" s="7"/>
     </row>
-    <row r="62" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="62" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P62" s="7"/>
     </row>
-    <row r="63" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="63" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P63" s="7"/>
     </row>
-    <row r="64" spans="6:16" x14ac:dyDescent="0.45">
+    <row r="64" spans="6:16" x14ac:dyDescent="0.2">
       <c r="P64" s="7"/>
     </row>
-    <row r="65" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="65" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P65" s="7"/>
     </row>
-    <row r="66" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="66" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P66" s="7"/>
     </row>
-    <row r="67" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="67" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P67" s="7"/>
     </row>
-    <row r="68" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="68" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P68" s="7"/>
     </row>
-    <row r="69" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="69" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P69" s="7"/>
     </row>
-    <row r="70" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="70" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P70" s="7"/>
     </row>
-    <row r="71" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="71" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P71" s="7"/>
     </row>
-    <row r="72" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="72" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P72" s="7"/>
     </row>
-    <row r="73" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="73" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P73" s="7"/>
     </row>
-    <row r="74" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="74" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P74" s="7"/>
     </row>
-    <row r="75" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="75" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P75" s="7"/>
     </row>
-    <row r="76" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="76" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P76" s="7"/>
     </row>
-    <row r="77" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="77" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P77" s="7"/>
     </row>
-    <row r="78" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="78" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P78" s="7"/>
     </row>
-    <row r="79" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="79" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P79" s="7"/>
     </row>
-    <row r="80" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="80" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P80" s="7"/>
     </row>
-    <row r="81" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="81" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P81" s="7"/>
     </row>
-    <row r="82" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="82" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P82" s="7"/>
     </row>
-    <row r="83" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="83" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P83" s="7"/>
     </row>
-    <row r="84" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="84" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P84" s="7"/>
     </row>
-    <row r="85" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="85" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P85" s="7"/>
     </row>
   </sheetData>
@@ -3619,17 +3621,17 @@
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>81</v>
       </c>
@@ -3638,7 +3640,7 @@
         <v>63.546386953382587</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>83</v>
       </c>
@@ -3649,7 +3651,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>85</v>
       </c>
@@ -3660,7 +3662,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>84</v>
       </c>
@@ -3671,7 +3673,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>86</v>
       </c>
@@ -3679,7 +3681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>87</v>
       </c>
@@ -3691,12 +3693,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>81</v>
       </c>
@@ -3705,7 +3707,7 @@
         <v>127.09277390676517</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>83</v>
       </c>
@@ -3713,7 +3715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>85</v>
       </c>
@@ -3721,7 +3723,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>93</v>
       </c>
@@ -3733,7 +3735,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>94</v>
       </c>
@@ -3745,7 +3747,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>84</v>
       </c>
@@ -3753,7 +3755,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>86</v>
       </c>
@@ -3761,7 +3763,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:4" ht="17" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
finished schematic, started panel BOM
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDC5D9F-5B8B-0645-AD90-D0CC344A75F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5663AA5A-DF20-C246-99E3-40625F875F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPL" sheetId="1" r:id="rId1"/>
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1767,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEB1EA-E152-4802-8ABB-B4D06F75C74E}">
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2879,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303E5587-B5A3-4B05-AB52-57C1D2A24CD5}">
   <dimension ref="B2:I11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>